<commit_message>
Update bảng kế  hoạch sau khi chỉnh sửa.xlsx
</commit_message>
<xml_diff>
--- a/bảng kế  hoạch sau khi chỉnh sửa.xlsx
+++ b/bảng kế  hoạch sau khi chỉnh sửa.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Chrome Download\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vo Tan Nguyen\Documents\GitHub\CODE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D87C1EB-5496-422C-8B72-BFD4DCD90D58}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90A4B0C4-B56E-4F6D-9838-1DE3FF6A27D4}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24990" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
   <si>
     <t>STT</t>
   </si>
@@ -121,13 +121,16 @@
   </si>
   <si>
     <t>viết hàm sử lý mergesort sau đó đệ quy. Debug lỗi cú pháp. Sữa lỗi nếu có</t>
+  </si>
+  <si>
+    <t>Bảng kết hoạch thực hiện đồ án Đề tài sắp xếp danh sách liên kết bằng Mersort</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,6 +159,13 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="30"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -177,7 +187,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -198,6 +208,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -515,7 +526,7 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -529,64 +540,43 @@
     <col min="8" max="8" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:8" ht="45.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="B1" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="5">
-        <v>43365</v>
-      </c>
-      <c r="H2" s="5">
-        <v>43365</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>7</v>
@@ -595,192 +585,196 @@
         <v>7</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G3" s="5">
-        <v>43368</v>
+        <v>43365</v>
       </c>
       <c r="H3" s="5">
-        <v>43368</v>
+        <v>43365</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="3"/>
+        <v>9</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="D4" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G4" s="5">
-        <v>43371</v>
+        <v>43368</v>
       </c>
       <c r="H4" s="5">
-        <v>43373</v>
+        <v>43368</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="5">
-        <v>43141</v>
-      </c>
-      <c r="F5" s="5">
-        <v>43200</v>
-      </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="3"/>
+        <v>10</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="5">
+        <v>43371</v>
+      </c>
+      <c r="H5" s="5">
+        <v>43373</v>
+      </c>
     </row>
     <row r="6" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3" t="s">
-        <v>7</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="3"/>
       <c r="E6" s="5">
-        <v>43291</v>
+        <v>43141</v>
       </c>
       <c r="F6" s="5">
-        <v>43322</v>
+        <v>43200</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="3"/>
     </row>
     <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>7</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E7" s="5">
-        <v>43414</v>
+        <v>43291</v>
       </c>
       <c r="F7" s="5">
-        <v>43444</v>
+        <v>43322</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8" s="3"/>
+      <c r="D8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="5">
+        <v>43414</v>
+      </c>
+      <c r="F8" s="5">
+        <v>43444</v>
+      </c>
+      <c r="G8" s="5"/>
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3" t="s">
-        <v>7</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="3"/>
       <c r="E10" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>7</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="C11" s="3"/>
       <c r="D11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="5">
-        <v>43142</v>
-      </c>
-      <c r="F11" s="5">
-        <v>43231</v>
+      <c r="E11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>7</v>
@@ -789,20 +783,35 @@
         <v>7</v>
       </c>
       <c r="E12" s="5">
-        <v>43262</v>
+        <v>43142</v>
       </c>
       <c r="F12" s="5">
-        <v>43262</v>
+        <v>43231</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+    <row r="13" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A13" s="7">
+        <v>11</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="5">
+        <v>43262</v>
+      </c>
+      <c r="F13" s="5">
+        <v>43262</v>
+      </c>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>

</xml_diff>

<commit_message>
cập nhập code và bảng kế hoạch 19/10/2018
</commit_message>
<xml_diff>
--- a/bảng kế  hoạch sau khi chỉnh sửa.xlsx
+++ b/bảng kế  hoạch sau khi chỉnh sửa.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vo Tan Nguyen\Documents\GitHub\CODE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90A4B0C4-B56E-4F6D-9838-1DE3FF6A27D4}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A12DF0EC-3C95-485E-83A9-50A46219FCCD}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24990" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -525,8 +525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -659,13 +659,17 @@
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="5">
-        <v>43141</v>
+        <v>43375</v>
       </c>
       <c r="F6" s="5">
-        <v>43200</v>
-      </c>
-      <c r="G6" s="5"/>
-      <c r="H6" s="3"/>
+        <v>43377</v>
+      </c>
+      <c r="G6" s="5">
+        <v>43375</v>
+      </c>
+      <c r="H6" s="5">
+        <v>43377</v>
+      </c>
     </row>
     <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
@@ -679,13 +683,17 @@
         <v>7</v>
       </c>
       <c r="E7" s="5">
-        <v>43291</v>
+        <v>43380</v>
       </c>
       <c r="F7" s="5">
-        <v>43322</v>
-      </c>
-      <c r="G7" s="5"/>
-      <c r="H7" s="3"/>
+        <v>43381</v>
+      </c>
+      <c r="G7" s="5">
+        <v>43380</v>
+      </c>
+      <c r="H7" s="5">
+        <v>43388</v>
+      </c>
     </row>
     <row r="8" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
@@ -706,7 +714,9 @@
       <c r="F8" s="5">
         <v>43444</v>
       </c>
-      <c r="G8" s="5"/>
+      <c r="G8" s="5">
+        <v>43390</v>
+      </c>
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>